<commit_message>
se sube docuemnto de hazasgos claves
</commit_message>
<xml_diff>
--- a/project_management/0. Lista de Documentos Proyecto.xlsx
+++ b/project_management/0. Lista de Documentos Proyecto.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeChaNiCoX\Desktop\Gerencia de Proyectos Ciencia de Datos\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mguerra\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D98655F-8008-43C9-BD1A-704795BE067B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F8B76F-C24F-414A-8E87-2CE91F6A2E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ListadoDocs" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,13 @@
     <sheet name="Riesgos" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ListadoDocs!$D$2:$H$27</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ListadoDocs!$D$2:$H$40</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -39,177 +42,177 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="144">
-  <si>
-    <t>repo</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>docs</t>
-  </si>
-  <si>
-    <t>notebooks</t>
-  </si>
-  <si>
-    <t>project_management</t>
-  </si>
-  <si>
-    <t>reports</t>
-  </si>
-  <si>
-    <t>src</t>
-  </si>
-  <si>
-    <t>data_description.md</t>
-  </si>
-  <si>
-    <t>Noticias.xlsx</t>
-  </si>
-  <si>
-    <t>methodology</t>
-  </si>
-  <si>
-    <t>roles</t>
-  </si>
-  <si>
-    <t>tools_and_environment</t>
-  </si>
-  <si>
-    <t>data_governance.md</t>
-  </si>
-  <si>
-    <t>data_pipeline_design.md</t>
-  </si>
-  <si>
-    <t>methodology.md</t>
-  </si>
-  <si>
-    <t>V1. Justificación de la Metodología.pdf</t>
-  </si>
-  <si>
-    <t>project_manager.md</t>
-  </si>
-  <si>
-    <t>roles.md</t>
-  </si>
-  <si>
-    <t>Roles.pdf</t>
-  </si>
-  <si>
-    <t>tools.md</t>
-  </si>
-  <si>
-    <t>notebooks_guide.md</t>
-  </si>
-  <si>
-    <t>Recolección y exploración del corpus de noticias V1.ipynb</t>
-  </si>
-  <si>
-    <t>project_plan.md</t>
-  </si>
-  <si>
-    <t>risk_assessment.md</t>
-  </si>
-  <si>
-    <t>stakeholder_analysis.md</t>
-  </si>
-  <si>
-    <t>V1. Plan de Proyecto.pdf</t>
-  </si>
-  <si>
-    <t>V2. Plan de Proyecto.pdf</t>
-  </si>
-  <si>
-    <t>data_quality</t>
-  </si>
-  <si>
-    <t>executive_summary</t>
-  </si>
-  <si>
-    <t>model_evaluation</t>
-  </si>
-  <si>
-    <t>data_quality.md</t>
-  </si>
-  <si>
-    <t>data_validation.md</t>
-  </si>
-  <si>
-    <t>Recolección y exploración del corpus de noticias V1.html</t>
-  </si>
-  <si>
-    <t>executive_summary.md</t>
-  </si>
-  <si>
-    <t>key_findings.md</t>
-  </si>
-  <si>
-    <t>model_evaluation.md</t>
-  </si>
-  <si>
-    <t>code_guidelines.md</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="160">
   <si>
     <t>PROYECTO: Recolección y Procesamiento de Noticias</t>
   </si>
   <si>
-    <t>Nivel 1</t>
-  </si>
-  <si>
-    <t>Nivel 2</t>
-  </si>
-  <si>
-    <t>Nivel 3</t>
-  </si>
-  <si>
-    <t>Nivel 4</t>
-  </si>
-  <si>
-    <t>Formato</t>
-  </si>
-  <si>
-    <t>md</t>
-  </si>
-  <si>
-    <t>xlsx</t>
-  </si>
-  <si>
-    <t>pdf</t>
-  </si>
-  <si>
-    <t>ipynb</t>
-  </si>
-  <si>
-    <t>html</t>
-  </si>
-  <si>
     <t>SCRUM</t>
-  </si>
-  <si>
-    <t>REPOSITORIO</t>
-  </si>
-  <si>
-    <t>GitHub</t>
-  </si>
-  <si>
-    <t>OneDrive</t>
-  </si>
-  <si>
-    <t>Trello</t>
   </si>
   <si>
     <t>ETAPAS
 CRISP-DM</t>
   </si>
   <si>
+    <t>REPOSITORIO</t>
+  </si>
+  <si>
+    <t>Nivel 1</t>
+  </si>
+  <si>
+    <t>Nivel 2</t>
+  </si>
+  <si>
+    <t>Nivel 3</t>
+  </si>
+  <si>
+    <t>Nivel 4</t>
+  </si>
+  <si>
+    <t>Formato</t>
+  </si>
+  <si>
     <t>Comprensión</t>
   </si>
   <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>repo</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>data_description.md</t>
+  </si>
+  <si>
+    <t>md</t>
+  </si>
+  <si>
+    <t>Noticias.xlsx</t>
+  </si>
+  <si>
+    <t>xlsx</t>
+  </si>
+  <si>
+    <t>docs</t>
+  </si>
+  <si>
+    <t>methodology</t>
+  </si>
+  <si>
+    <t>data_governance.md</t>
+  </si>
+  <si>
+    <t>data_pipeline_design.md</t>
+  </si>
+  <si>
+    <t>methodology.md</t>
+  </si>
+  <si>
+    <t>V1. Justificación de la Metodología.pdf</t>
+  </si>
+  <si>
+    <t>pdf</t>
+  </si>
+  <si>
+    <t>roles</t>
+  </si>
+  <si>
+    <t>project_manager.md</t>
+  </si>
+  <si>
+    <t>roles.md</t>
+  </si>
+  <si>
+    <t>Roles.pdf</t>
+  </si>
+  <si>
     <t>Preparación</t>
   </si>
   <si>
+    <t>tools_and_environment</t>
+  </si>
+  <si>
+    <t>tools.md</t>
+  </si>
+  <si>
+    <t>notebooks</t>
+  </si>
+  <si>
+    <t>notebooks_guide.md</t>
+  </si>
+  <si>
+    <t>Recolección y exploración del corpus de noticias V1.ipynb</t>
+  </si>
+  <si>
+    <t>ipynb</t>
+  </si>
+  <si>
+    <t>project_management</t>
+  </si>
+  <si>
+    <t>project_plan.md</t>
+  </si>
+  <si>
+    <t>risk_assessment.md</t>
+  </si>
+  <si>
+    <t>stakeholder_analysis.md</t>
+  </si>
+  <si>
+    <t>V1. Plan de Proyecto.pdf</t>
+  </si>
+  <si>
+    <t>V2. Plan de Proyecto.pdf</t>
+  </si>
+  <si>
+    <t>reports</t>
+  </si>
+  <si>
+    <t>data_quality</t>
+  </si>
+  <si>
+    <t>data_quality.md</t>
+  </si>
+  <si>
+    <t>data_validation.md</t>
+  </si>
+  <si>
+    <t>Recolección y exploración del corpus de noticias V1.html</t>
+  </si>
+  <si>
+    <t>html</t>
+  </si>
+  <si>
+    <t>executive_summary</t>
+  </si>
+  <si>
+    <t>executive_summary.md</t>
+  </si>
+  <si>
+    <t>key_findings.md</t>
+  </si>
+  <si>
+    <t>model_evaluation</t>
+  </si>
+  <si>
+    <t>model_evaluation.md</t>
+  </si>
+  <si>
+    <t>src</t>
+  </si>
+  <si>
+    <t>code_guidelines.md</t>
+  </si>
+  <si>
+    <t>OneDrive</t>
+  </si>
+  <si>
+    <t>Trello</t>
+  </si>
+  <si>
     <t>Canva</t>
   </si>
   <si>
@@ -411,30 +414,30 @@
     <t>R3</t>
   </si>
   <si>
+    <t>Problemas técnicos o computacionales</t>
+  </si>
+  <si>
+    <t>Tecnológico</t>
+  </si>
+  <si>
     <t>R4</t>
   </si>
   <si>
-    <t>Problemas técnicos o computacionales</t>
-  </si>
-  <si>
-    <t>Tecnológico</t>
+    <t>Falta de coordinación en el equipo</t>
+  </si>
+  <si>
+    <t>Organizacional</t>
   </si>
   <si>
     <t>R5</t>
   </si>
   <si>
-    <t>Falta de coordinación en el equipo</t>
-  </si>
-  <si>
-    <t>Organizacional</t>
+    <t>Falta de precisión del modelo</t>
   </si>
   <si>
     <t>R6</t>
   </si>
   <si>
-    <t>Falta de precisión del modelo</t>
-  </si>
-  <si>
     <t>Retrasos en la documentación y presentación</t>
   </si>
   <si>
@@ -472,6 +475,54 @@
   </si>
   <si>
     <t>Asignar tareas específicas para la documentación desde el inicio y realizar revisiones continuas.</t>
+  </si>
+  <si>
+    <t>Gobernanza de Datos.docx</t>
+  </si>
+  <si>
+    <t>docx</t>
+  </si>
+  <si>
+    <t>Herramientas y entornos de Trabajo.docx</t>
+  </si>
+  <si>
+    <t>Limpieza, tokenización y vectorización con LSTM V2.ipynb</t>
+  </si>
+  <si>
+    <t>modelado</t>
+  </si>
+  <si>
+    <t>Ejecucion de Modelos Neuronales V3.ipynb</t>
+  </si>
+  <si>
+    <t>V3. Plan de Proyecto.pdf</t>
+  </si>
+  <si>
+    <t>Análisis de Stakeholders.docx</t>
+  </si>
+  <si>
+    <t>Gestión Scrum V1.xlsx</t>
+  </si>
+  <si>
+    <t>Plan de Comunicaciones.docx</t>
+  </si>
+  <si>
+    <t>0. Lista de Documentos Proyecto.xlsx</t>
+  </si>
+  <si>
+    <t>Limpieza, tokenización y vectorización con LSTM V2 Resultados.html</t>
+  </si>
+  <si>
+    <t>Ejecucion de Modelos Neuronales V3.html</t>
+  </si>
+  <si>
+    <t>Hagazgos Claves.pdf</t>
+  </si>
+  <si>
+    <t>Reporte Ejecutivo.pdf</t>
+  </si>
+  <si>
+    <t>evalucion</t>
   </si>
 </sst>
 </file>
@@ -695,15 +746,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -730,6 +772,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1033,13 +1084,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="18.7109375" style="1" customWidth="1"/>
@@ -1053,764 +1104,958 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="11"/>
+      <c r="A1" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>49</v>
+        <v>3</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>40</v>
+        <v>6</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>16</v>
+        <v>144</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="G13" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="G14" s="2" t="s">
-        <v>21</v>
+        <v>146</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2" t="s">
-        <v>24</v>
+        <v>147</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>148</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="2" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="2" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F20" s="2"/>
       <c r="G20" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C21" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F21" s="2"/>
       <c r="G21" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C22" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F22" s="2"/>
       <c r="G22" s="2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C23" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F23" s="2"/>
       <c r="G23" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C24" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>28</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F24" s="2"/>
       <c r="G24" s="2" t="s">
-        <v>34</v>
+        <v>150</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C25" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F25" s="2"/>
       <c r="G25" s="2" t="s">
-        <v>35</v>
+        <v>151</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>43</v>
+        <v>145</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C26" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>36</v>
+        <v>152</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+      <c r="B27" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C27" s="2" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>6</v>
+        <v>35</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2" t="s">
-        <v>32</v>
+        <v>153</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>47</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C28" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="G28" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C29" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="G30" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H30" s="2"/>
+        <v>44</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
+      <c r="B31" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
+      <c r="B32" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
+      <c r="B33" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
+      <c r="B34" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
+      <c r="B35" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
+      <c r="B36" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
+      <c r="B37" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
-      <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
+      <c r="B38" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
+      <c r="C39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
+      <c r="G39" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="B40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
+      <c r="G40" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
+      <c r="B41" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
+      <c r="G41" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
+      <c r="B42" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
+      <c r="G42" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
@@ -1825,7 +2070,9 @@
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
+      <c r="C44" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
@@ -1835,7 +2082,9 @@
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="C45" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
@@ -1845,11 +2094,15 @@
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
+      <c r="C46" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
+      <c r="G46" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="H46" s="2"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1912,8 +2165,168 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="2"/>
+      <c r="G55" s="2"/>
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="2"/>
+      <c r="B58" s="2"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="2"/>
+      <c r="B59" s="2"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="2"/>
+      <c r="B61" s="2"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="2"/>
+      <c r="B62" s="2"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="2"/>
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="2"/>
+      <c r="B63" s="2"/>
+      <c r="C63" s="2"/>
+      <c r="D63" s="2"/>
+      <c r="E63" s="2"/>
+      <c r="F63" s="2"/>
+      <c r="G63" s="2"/>
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="2"/>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
+      <c r="D64" s="2"/>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
+      <c r="G64" s="2"/>
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="2"/>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="2"/>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="2"/>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2"/>
+      <c r="D68" s="2"/>
+      <c r="E68" s="2"/>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="D2:H27" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="D2:H40" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="1">
     <mergeCell ref="A1:H1"/>
   </mergeCells>
@@ -1930,120 +2343,120 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="5" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="9" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="8" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="9" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="9" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="9" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2061,172 +2474,172 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="5" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="14" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="12" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="12" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="10" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="14" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="18" t="s">
+      <c r="B15" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="16" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="16" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="9" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
+    <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="9" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="9" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="9" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="9" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2244,7 +2657,7 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.7109375" customWidth="1"/>
@@ -2257,198 +2670,198 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="13" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="9" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="17" t="s">
         <v>122</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="D5" s="12" t="s">
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E6" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F6" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H9" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="H10" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="H11" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="H12" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="H13" s="17" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="12" t="s">
+      <c r="I13" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="H14" s="17" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="C7" s="12" t="s">
+      <c r="I14" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="H15" s="17" t="s">
         <v>130</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H9" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="J9" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="H10" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="H11" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="H12" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="J12" s="12" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="H13" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="H14" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>141</v>
-      </c>
-      <c r="J14" s="12" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="H15" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="I15" s="12" t="s">
+      <c r="I15" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="J15" s="9" t="s">
         <v>142</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se sube docuemnto informe ejecutivo
</commit_message>
<xml_diff>
--- a/project_management/0. Lista de Documentos Proyecto.xlsx
+++ b/project_management/0. Lista de Documentos Proyecto.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mguerra\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mguerra\Documents\Documentos\ESTUDIO\3 semestre\GWEWNCIA PROYECTOS\repo\template_pcd\project_management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F8B76F-C24F-414A-8E87-2CE91F6A2E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFCB1A5-19F6-485F-86A2-3CF3150070FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,10 +519,10 @@
     <t>Hagazgos Claves.pdf</t>
   </si>
   <si>
-    <t>Reporte Ejecutivo.pdf</t>
-  </si>
-  <si>
     <t>evalucion</t>
+  </si>
+  <si>
+    <t>Reporte Ejecutivo Grupo 1 Clasificacion Noticias.pdf</t>
   </si>
 </sst>
 </file>
@@ -1087,7 +1087,7 @@
   <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,7 +1854,7 @@
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>10</v>
@@ -1878,7 +1878,7 @@
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>10</v>
@@ -1902,7 +1902,7 @@
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>10</v>
@@ -1926,7 +1926,7 @@
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>10</v>
@@ -1941,7 +1941,7 @@
         <v>47</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>23</v>
@@ -1950,7 +1950,7 @@
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>10</v>

</xml_diff>